<commit_message>
added files for docmagic
</commit_message>
<xml_diff>
--- a/data/577 Projects/2014-2015/Transaction_Evaluation.xlsx
+++ b/data/577 Projects/2014-2015/Transaction_Evaluation.xlsx
@@ -3,18 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0D58F58D-E608-46AC-AE04-B58AEE552E15}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FDC4D4BD-E747-4261-8127-61356123DE10}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="F14a_women_at_work_website_rede" sheetId="1" r:id="rId1"/>
-    <sheet name="F14a_soccer_data_web_crawler" sheetId="2" r:id="rId2"/>
-    <sheet name="F14a_black_professionals_net" sheetId="3" r:id="rId3"/>
-    <sheet name="F14a_gotrla" sheetId="4" r:id="rId4"/>
-    <sheet name="F14a_sharethetraining_com" sheetId="5" r:id="rId5"/>
+    <sheet name="Evaluation_Restults" sheetId="6" r:id="rId1"/>
+    <sheet name="F14a_women_at_work_website_rede" sheetId="1" r:id="rId2"/>
+    <sheet name="F14a_soccer_data_web_crawler" sheetId="2" r:id="rId3"/>
+    <sheet name="F14a_black_professionals_net" sheetId="3" r:id="rId4"/>
+    <sheet name="F14a_gotrla" sheetId="4" r:id="rId5"/>
+    <sheet name="F14a_sharethetraining_com" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1415" uniqueCount="641">
   <si>
     <t>Use Case</t>
   </si>
@@ -2535,6 +2536,36 @@
   </si>
   <si>
     <t>Part4</t>
+  </si>
+  <si>
+    <t>F14a_soccer_data_web_crawler</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Identified</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>F14a_women_at_work_website_rede</t>
+  </si>
+  <si>
+    <t>F14a_black_professionals_net</t>
+  </si>
+  <si>
+    <t>F14a_gotrla</t>
+  </si>
+  <si>
+    <t>F14a_sharethetraining_com</t>
+  </si>
+  <si>
+    <t>avg.</t>
   </si>
 </sst>
 </file>
@@ -2858,6 +2889,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3108E38A-7D26-413F-B6A8-F0D5B27CE7BB}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>632</v>
+      </c>
+      <c r="B1" t="s">
+        <v>633</v>
+      </c>
+      <c r="C1" t="s">
+        <v>634</v>
+      </c>
+      <c r="D1" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>636</v>
+      </c>
+      <c r="B2">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>39</v>
+      </c>
+      <c r="D2">
+        <f>28/39</f>
+        <v>0.71794871794871795</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>631</v>
+      </c>
+      <c r="B3">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <f>33/50</f>
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>637</v>
+      </c>
+      <c r="B4">
+        <v>139</v>
+      </c>
+      <c r="C4">
+        <v>188</v>
+      </c>
+      <c r="D4">
+        <f>139/188</f>
+        <v>0.73936170212765961</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>638</v>
+      </c>
+      <c r="B5">
+        <v>67</v>
+      </c>
+      <c r="C5">
+        <v>82</v>
+      </c>
+      <c r="D5">
+        <f>67/82</f>
+        <v>0.81707317073170727</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>639</v>
+      </c>
+      <c r="B6">
+        <v>52</v>
+      </c>
+      <c r="C6">
+        <v>61</v>
+      </c>
+      <c r="D6">
+        <f>52/61</f>
+        <v>0.85245901639344257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="C7" t="s">
+        <v>640</v>
+      </c>
+      <c r="D7">
+        <f>AVERAGE(D2:D6)</f>
+        <v>0.75736852144030542</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
@@ -3284,11 +3428,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -3774,11 +3918,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A112" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -5925,11 +6069,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -7060,12 +7204,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>